<commit_message>
modify a print result
</commit_message>
<xml_diff>
--- a/months/jan23/jan23_results.xlsx
+++ b/months/jan23/jan23_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,6 +453,116 @@
           <t>a:bottle</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>a:sleeptime</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>a:dreams</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>z:stroll</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>z:sleeptime</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>z:teeth</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>z:edu</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>z:tele</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>h:vacuum</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>h:kitchen</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>e:plan</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>e:hygiene</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>e:siesta</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>e:dev</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>e:sleeptime</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>e:diet</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>e:meals</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>l:siesta</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>l:teeth</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>l:sleeptime</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>l:alarm</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>l:diet</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>l:meals</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -466,6 +576,72 @@
       </c>
       <c r="D2" t="n">
         <v>75</v>
+      </c>
+      <c r="E2" t="n">
+        <v>25</v>
+      </c>
+      <c r="F2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="V2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>25</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -481,6 +657,72 @@
       <c r="D3" t="n">
         <v>25</v>
       </c>
+      <c r="E3" t="n">
+        <v>75</v>
+      </c>
+      <c r="F3" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-50</v>
+      </c>
+      <c r="H3" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="L3" t="n">
+        <v>125</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-50</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>-70</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -495,6 +737,72 @@
       <c r="D4" t="n">
         <v>60</v>
       </c>
+      <c r="E4" t="n">
+        <v>180</v>
+      </c>
+      <c r="F4" t="n">
+        <v>50</v>
+      </c>
+      <c r="G4" t="n">
+        <v>50</v>
+      </c>
+      <c r="H4" t="n">
+        <v>90</v>
+      </c>
+      <c r="I4" t="n">
+        <v>50</v>
+      </c>
+      <c r="J4" t="n">
+        <v>50</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-50</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-50</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -509,6 +817,72 @@
       <c r="D5" t="n">
         <v>90</v>
       </c>
+      <c r="E5" t="n">
+        <v>20</v>
+      </c>
+      <c r="F5" t="n">
+        <v>50</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>200</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>50</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>50</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>50</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -523,6 +897,72 @@
       <c r="D6" t="n">
         <v>40</v>
       </c>
+      <c r="E6" t="n">
+        <v>30</v>
+      </c>
+      <c r="F6" t="n">
+        <v>50</v>
+      </c>
+      <c r="G6" t="n">
+        <v>50</v>
+      </c>
+      <c r="H6" t="n">
+        <v>54</v>
+      </c>
+      <c r="I6" t="n">
+        <v>50</v>
+      </c>
+      <c r="J6" t="n">
+        <v>50</v>
+      </c>
+      <c r="K6" t="n">
+        <v>50</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>50</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>-105</v>
+      </c>
+      <c r="X6" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -537,6 +977,72 @@
       <c r="D7" t="n">
         <v>40</v>
       </c>
+      <c r="E7" t="n">
+        <v>30</v>
+      </c>
+      <c r="F7" t="n">
+        <v>50</v>
+      </c>
+      <c r="G7" t="n">
+        <v>50</v>
+      </c>
+      <c r="H7" t="n">
+        <v>60</v>
+      </c>
+      <c r="I7" t="n">
+        <v>50</v>
+      </c>
+      <c r="J7" t="n">
+        <v>50</v>
+      </c>
+      <c r="K7" t="n">
+        <v>50</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-50</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>50</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>-110</v>
+      </c>
+      <c r="X7" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -551,6 +1057,72 @@
       <c r="D8" t="n">
         <v>30</v>
       </c>
+      <c r="E8" t="n">
+        <v>120</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>30</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>50</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>50</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>25</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -565,6 +1137,72 @@
       <c r="D9" t="n">
         <v>20</v>
       </c>
+      <c r="E9" t="n">
+        <v>15</v>
+      </c>
+      <c r="F9" t="n">
+        <v>50</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-50</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>50</v>
+      </c>
+      <c r="J9" t="n">
+        <v>50</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-50</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>50</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -579,6 +1217,72 @@
       <c r="D10" t="n">
         <v>20</v>
       </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>50</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-50</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-50</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>50</v>
+      </c>
+      <c r="L10" t="n">
+        <v>20</v>
+      </c>
+      <c r="M10" t="n">
+        <v>50</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" t="n">
+        <v>-30</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -593,6 +1297,72 @@
       <c r="D11" t="n">
         <v>0</v>
       </c>
+      <c r="E11" t="n">
+        <v>50</v>
+      </c>
+      <c r="F11" t="n">
+        <v>50</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-50</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>50</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>25</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -607,6 +1377,72 @@
       <c r="D12" t="n">
         <v>0</v>
       </c>
+      <c r="E12" t="n">
+        <v>60</v>
+      </c>
+      <c r="F12" t="n">
+        <v>50</v>
+      </c>
+      <c r="G12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H12" t="n">
+        <v>30</v>
+      </c>
+      <c r="I12" t="n">
+        <v>50</v>
+      </c>
+      <c r="J12" t="n">
+        <v>50</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" t="n">
+        <v>50</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -621,6 +1457,72 @@
       <c r="D13" t="n">
         <v>20</v>
       </c>
+      <c r="E13" t="n">
+        <v>40</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>50</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>-50</v>
+      </c>
+      <c r="J13" t="n">
+        <v>50</v>
+      </c>
+      <c r="K13" t="n">
+        <v>-50</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -635,6 +1537,72 @@
       <c r="D14" t="n">
         <v>0</v>
       </c>
+      <c r="E14" t="n">
+        <v>120</v>
+      </c>
+      <c r="F14" t="n">
+        <v>50</v>
+      </c>
+      <c r="G14" t="n">
+        <v>50</v>
+      </c>
+      <c r="H14" t="n">
+        <v>40</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -649,6 +1617,72 @@
       <c r="D15" t="n">
         <v>20</v>
       </c>
+      <c r="E15" t="n">
+        <v>5</v>
+      </c>
+      <c r="F15" t="n">
+        <v>50</v>
+      </c>
+      <c r="G15" t="n">
+        <v>50</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>50</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>25</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -663,6 +1697,72 @@
       <c r="D16" t="n">
         <v>0</v>
       </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-50</v>
+      </c>
+      <c r="H16" t="n">
+        <v>80</v>
+      </c>
+      <c r="I16" t="n">
+        <v>-50</v>
+      </c>
+      <c r="J16" t="n">
+        <v>50</v>
+      </c>
+      <c r="K16" t="n">
+        <v>50</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>50</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -677,6 +1777,72 @@
       <c r="D17" t="n">
         <v>0</v>
       </c>
+      <c r="E17" t="n">
+        <v>10</v>
+      </c>
+      <c r="F17" t="n">
+        <v>25</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>25</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" t="n">
+        <v>25</v>
+      </c>
+      <c r="V17" t="n">
+        <v>25</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -691,6 +1857,72 @@
       <c r="D18" t="n">
         <v>20</v>
       </c>
+      <c r="E18" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="F18" t="n">
+        <v>25</v>
+      </c>
+      <c r="G18" t="n">
+        <v>25</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>25</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>25</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>25</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" t="n">
+        <v>50</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" t="n">
+        <v>-40</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -705,6 +1937,72 @@
       <c r="D19" t="n">
         <v>20</v>
       </c>
+      <c r="E19" t="n">
+        <v>10</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>25</v>
+      </c>
+      <c r="H19" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="I19" t="n">
+        <v>25</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>25</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>-50</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" t="n">
+        <v>50</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0</v>
+      </c>
+      <c r="W19" t="n">
+        <v>-10</v>
+      </c>
+      <c r="X19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>25</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -719,6 +2017,72 @@
       <c r="D20" t="n">
         <v>30</v>
       </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>25</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>25</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="n">
+        <v>-25</v>
+      </c>
+      <c r="V20" t="n">
+        <v>25</v>
+      </c>
+      <c r="W20" t="n">
+        <v>0</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -733,6 +2097,72 @@
       <c r="D21" t="n">
         <v>0</v>
       </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>25</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-50</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>25</v>
+      </c>
+      <c r="J21" t="n">
+        <v>25</v>
+      </c>
+      <c r="K21" t="n">
+        <v>25</v>
+      </c>
+      <c r="L21" t="n">
+        <v>50</v>
+      </c>
+      <c r="M21" t="n">
+        <v>25</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" t="n">
+        <v>50</v>
+      </c>
+      <c r="V21" t="n">
+        <v>-50</v>
+      </c>
+      <c r="W21" t="n">
+        <v>-20</v>
+      </c>
+      <c r="X21" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>25</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -747,6 +2177,72 @@
       <c r="D22" t="n">
         <v>0</v>
       </c>
+      <c r="E22" t="n">
+        <v>200</v>
+      </c>
+      <c r="F22" t="n">
+        <v>50</v>
+      </c>
+      <c r="G22" t="n">
+        <v>50</v>
+      </c>
+      <c r="H22" t="n">
+        <v>90</v>
+      </c>
+      <c r="I22" t="n">
+        <v>50</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>40</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0</v>
+      </c>
+      <c r="V22" t="n">
+        <v>0</v>
+      </c>
+      <c r="W22" t="n">
+        <v>0</v>
+      </c>
+      <c r="X22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -761,6 +2257,72 @@
       <c r="D23" t="n">
         <v>0</v>
       </c>
+      <c r="E23" t="n">
+        <v>20</v>
+      </c>
+      <c r="F23" t="n">
+        <v>50</v>
+      </c>
+      <c r="G23" t="n">
+        <v>-50</v>
+      </c>
+      <c r="H23" t="n">
+        <v>84</v>
+      </c>
+      <c r="I23" t="n">
+        <v>-50</v>
+      </c>
+      <c r="J23" t="n">
+        <v>50</v>
+      </c>
+      <c r="K23" t="n">
+        <v>-50</v>
+      </c>
+      <c r="L23" t="n">
+        <v>20</v>
+      </c>
+      <c r="M23" t="n">
+        <v>50</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0</v>
+      </c>
+      <c r="U23" t="n">
+        <v>0</v>
+      </c>
+      <c r="V23" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" t="n">
+        <v>0</v>
+      </c>
+      <c r="X23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -775,6 +2337,72 @@
       <c r="D24" t="n">
         <v>10</v>
       </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>-50</v>
+      </c>
+      <c r="H24" t="n">
+        <v>15</v>
+      </c>
+      <c r="I24" t="n">
+        <v>25</v>
+      </c>
+      <c r="J24" t="n">
+        <v>25</v>
+      </c>
+      <c r="K24" t="n">
+        <v>25</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>25</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" t="n">
+        <v>-80</v>
+      </c>
+      <c r="X24" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>25</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -789,6 +2417,72 @@
       <c r="D25" t="n">
         <v>20</v>
       </c>
+      <c r="E25" t="n">
+        <v>27</v>
+      </c>
+      <c r="F25" t="n">
+        <v>25</v>
+      </c>
+      <c r="G25" t="n">
+        <v>-50</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>25</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>25</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
+        <v>25</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0</v>
+      </c>
+      <c r="U25" t="n">
+        <v>25</v>
+      </c>
+      <c r="V25" t="n">
+        <v>-50</v>
+      </c>
+      <c r="W25" t="n">
+        <v>-50</v>
+      </c>
+      <c r="X25" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>25</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -803,6 +2497,72 @@
       <c r="D26" t="n">
         <v>15</v>
       </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>25</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>25</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="n">
+        <v>25</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0</v>
+      </c>
+      <c r="U26" t="n">
+        <v>0</v>
+      </c>
+      <c r="V26" t="n">
+        <v>25</v>
+      </c>
+      <c r="W26" t="n">
+        <v>0</v>
+      </c>
+      <c r="X26" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -815,6 +2575,72 @@
         <v>4</v>
       </c>
       <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>30</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>-50</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>25</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>25</v>
+      </c>
+      <c r="L27" t="n">
+        <v>20</v>
+      </c>
+      <c r="M27" t="n">
+        <v>25</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0</v>
+      </c>
+      <c r="U27" t="n">
+        <v>0</v>
+      </c>
+      <c r="V27" t="n">
+        <v>-50</v>
+      </c>
+      <c r="W27" t="n">
+        <v>-120</v>
+      </c>
+      <c r="X27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>25</v>
+      </c>
+      <c r="Z27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -831,6 +2657,72 @@
       <c r="D28" t="n">
         <v>10</v>
       </c>
+      <c r="E28" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="F28" t="n">
+        <v>25</v>
+      </c>
+      <c r="G28" t="n">
+        <v>-50</v>
+      </c>
+      <c r="H28" t="n">
+        <v>19</v>
+      </c>
+      <c r="I28" t="n">
+        <v>25</v>
+      </c>
+      <c r="J28" t="n">
+        <v>25</v>
+      </c>
+      <c r="K28" t="n">
+        <v>25</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="n">
+        <v>25</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" t="n">
+        <v>-50</v>
+      </c>
+      <c r="X28" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>25</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -845,6 +2737,72 @@
       <c r="D29" t="n">
         <v>30</v>
       </c>
+      <c r="E29" t="n">
+        <v>60</v>
+      </c>
+      <c r="F29" t="n">
+        <v>50</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>50</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" t="n">
+        <v>50</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0</v>
+      </c>
+      <c r="U29" t="n">
+        <v>0</v>
+      </c>
+      <c r="V29" t="n">
+        <v>0</v>
+      </c>
+      <c r="W29" t="n">
+        <v>0</v>
+      </c>
+      <c r="X29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -859,6 +2817,72 @@
       <c r="D30" t="n">
         <v>20</v>
       </c>
+      <c r="E30" t="n">
+        <v>120</v>
+      </c>
+      <c r="F30" t="n">
+        <v>50</v>
+      </c>
+      <c r="G30" t="n">
+        <v>50</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>-50</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>50</v>
+      </c>
+      <c r="L30" t="n">
+        <v>20</v>
+      </c>
+      <c r="M30" t="n">
+        <v>-50</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0</v>
+      </c>
+      <c r="W30" t="n">
+        <v>-75</v>
+      </c>
+      <c r="X30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -873,6 +2897,72 @@
       <c r="D31" t="n">
         <v>0</v>
       </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>-50</v>
+      </c>
+      <c r="H31" t="n">
+        <v>20</v>
+      </c>
+      <c r="I31" t="n">
+        <v>25</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>25</v>
+      </c>
+      <c r="L31" t="n">
+        <v>50</v>
+      </c>
+      <c r="M31" t="n">
+        <v>25</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0</v>
+      </c>
+      <c r="V31" t="n">
+        <v>-50</v>
+      </c>
+      <c r="W31" t="n">
+        <v>-20</v>
+      </c>
+      <c r="X31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -886,6 +2976,72 @@
       </c>
       <c r="D32" t="n">
         <v>15</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>25</v>
+      </c>
+      <c r="G32" t="n">
+        <v>25</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>25</v>
+      </c>
+      <c r="J32" t="n">
+        <v>25</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0</v>
+      </c>
+      <c r="V32" t="n">
+        <v>25</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0</v>
+      </c>
+      <c r="X32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="33">
@@ -901,6 +3057,72 @@
       <c r="D33" t="n">
         <v>630</v>
       </c>
+      <c r="E33" t="n">
+        <v>1270</v>
+      </c>
+      <c r="F33" t="n">
+        <v>1025</v>
+      </c>
+      <c r="G33" t="n">
+        <v>-75</v>
+      </c>
+      <c r="H33" t="n">
+        <v>893</v>
+      </c>
+      <c r="I33" t="n">
+        <v>512.5</v>
+      </c>
+      <c r="J33" t="n">
+        <v>662.5</v>
+      </c>
+      <c r="K33" t="n">
+        <v>362.5</v>
+      </c>
+      <c r="L33" t="n">
+        <v>345</v>
+      </c>
+      <c r="M33" t="n">
+        <v>462.5</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0</v>
+      </c>
+      <c r="U33" t="n">
+        <v>312.5</v>
+      </c>
+      <c r="V33" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="W33" t="n">
+        <v>-780</v>
+      </c>
+      <c r="X33" t="n">
+        <v>115</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>1212.5</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>375</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>